<commit_message>
correction problèmes génération fichiers json
</commit_message>
<xml_diff>
--- a/projetS5/public/INFO/2018-2019/ADMIN/LISTES/INFO_2018-2019_ADMIN_LISTES_S1.xlsx
+++ b/projetS5/public/INFO/2018-2019/ADMIN/LISTES/INFO_2018-2019_ADMIN_LISTES_S1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdcde\Music\PROJET S5 LPDIOC GESTION ETUDIANT\GestionEtudiants2018\projetS5\public\INFO\2018-2019\ADMIN\LISTES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AFD7CD-27C8-4DB7-96CF-40173A3832D5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9845B431-76D7-4349-9FF9-E8F9C8FA7A91}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{B8C28436-09AF-4DF1-8BB7-62D1DDCC6DAF}"/>
   </bookViews>
@@ -856,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A245600-A942-4A9C-BA06-5CDF207C8B57}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="I64" sqref="I64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -898,7 +898,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>20170926</v>
+        <v>20150926</v>
       </c>
       <c r="B3" t="s">
         <v>95</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>20170927</v>
+        <v>20150927</v>
       </c>
       <c r="B4" t="s">
         <v>96</v>
@@ -956,7 +956,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>20170928</v>
+        <v>20150928</v>
       </c>
       <c r="B5" t="s">
         <v>97</v>
@@ -985,7 +985,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>20170929</v>
+        <v>20150929</v>
       </c>
       <c r="B6" t="s">
         <v>98</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>20170930</v>
+        <v>20150930</v>
       </c>
       <c r="B7" t="s">
         <v>99</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>20170931</v>
+        <v>20150931</v>
       </c>
       <c r="B8" t="s">
         <v>100</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>20170932</v>
+        <v>20150932</v>
       </c>
       <c r="B9" t="s">
         <v>101</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>20170933</v>
+        <v>20150933</v>
       </c>
       <c r="B10" t="s">
         <v>102</v>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>20170934</v>
+        <v>20150934</v>
       </c>
       <c r="B11" t="s">
         <v>103</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>20170935</v>
+        <v>20150935</v>
       </c>
       <c r="B12" t="s">
         <v>104</v>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>20170936</v>
+        <v>20150936</v>
       </c>
       <c r="B13" t="s">
         <v>105</v>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>20170937</v>
+        <v>20150937</v>
       </c>
       <c r="B14" t="s">
         <v>106</v>
@@ -1246,7 +1246,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>20170938</v>
+        <v>20150938</v>
       </c>
       <c r="B15" t="s">
         <v>107</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>20170939</v>
+        <v>20150939</v>
       </c>
       <c r="B16" t="s">
         <v>108</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>20170940</v>
+        <v>20150940</v>
       </c>
       <c r="B17" t="s">
         <v>109</v>
@@ -1333,7 +1333,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>20170941</v>
+        <v>20150941</v>
       </c>
       <c r="B18" t="s">
         <v>110</v>
@@ -1362,7 +1362,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>20170942</v>
+        <v>20150942</v>
       </c>
       <c r="B19" t="s">
         <v>111</v>
@@ -1391,7 +1391,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>20170943</v>
+        <v>20150943</v>
       </c>
       <c r="B20" t="s">
         <v>112</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>20170944</v>
+        <v>20150944</v>
       </c>
       <c r="B21" t="s">
         <v>113</v>
@@ -1449,7 +1449,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>20170945</v>
+        <v>20150945</v>
       </c>
       <c r="B22" t="s">
         <v>114</v>
@@ -1478,7 +1478,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>20170946</v>
+        <v>20150946</v>
       </c>
       <c r="B23" t="s">
         <v>115</v>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>20170947</v>
+        <v>20150947</v>
       </c>
       <c r="B24" t="s">
         <v>116</v>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>20170948</v>
+        <v>20150948</v>
       </c>
       <c r="B25" t="s">
         <v>117</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>20170949</v>
+        <v>20150949</v>
       </c>
       <c r="B26" t="s">
         <v>118</v>
@@ -1594,7 +1594,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>20170950</v>
+        <v>20150950</v>
       </c>
       <c r="B27" t="s">
         <v>119</v>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>20170951</v>
+        <v>20150951</v>
       </c>
       <c r="B28" t="s">
         <v>120</v>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>20170952</v>
+        <v>20150952</v>
       </c>
       <c r="B29" t="s">
         <v>121</v>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>20170953</v>
+        <v>20150953</v>
       </c>
       <c r="B30" t="s">
         <v>122</v>
@@ -1710,7 +1710,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>20170954</v>
+        <v>20150954</v>
       </c>
       <c r="B31" t="s">
         <v>122</v>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>20170955</v>
+        <v>20150955</v>
       </c>
       <c r="B32" t="s">
         <v>123</v>
@@ -1768,7 +1768,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>20170956</v>
+        <v>20150956</v>
       </c>
       <c r="B33" t="s">
         <v>124</v>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>20170957</v>
+        <v>20150957</v>
       </c>
       <c r="B34" t="s">
         <v>125</v>
@@ -1826,7 +1826,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>20170958</v>
+        <v>20150958</v>
       </c>
       <c r="B35" t="s">
         <v>126</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>20170959</v>
+        <v>20150959</v>
       </c>
       <c r="B36" t="s">
         <v>127</v>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>20170960</v>
+        <v>20150960</v>
       </c>
       <c r="B37" t="s">
         <v>128</v>
@@ -1913,7 +1913,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>20170961</v>
+        <v>20150961</v>
       </c>
       <c r="B38" t="s">
         <v>129</v>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>20170962</v>
+        <v>20150962</v>
       </c>
       <c r="B39" t="s">
         <v>130</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>20170963</v>
+        <v>20150963</v>
       </c>
       <c r="B40" t="s">
         <v>131</v>
@@ -2000,7 +2000,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>20170964</v>
+        <v>20150964</v>
       </c>
       <c r="B41" t="s">
         <v>132</v>
@@ -2029,7 +2029,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>20170965</v>
+        <v>20150965</v>
       </c>
       <c r="B42" t="s">
         <v>133</v>
@@ -2058,7 +2058,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>20170966</v>
+        <v>20150966</v>
       </c>
       <c r="B43" t="s">
         <v>134</v>
@@ -2087,7 +2087,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>20170967</v>
+        <v>20150967</v>
       </c>
       <c r="B44" t="s">
         <v>135</v>
@@ -2116,7 +2116,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>20170968</v>
+        <v>20150968</v>
       </c>
       <c r="B45" t="s">
         <v>136</v>
@@ -2145,7 +2145,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>20170969</v>
+        <v>20150969</v>
       </c>
       <c r="B46" t="s">
         <v>137</v>
@@ -2174,7 +2174,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>20170970</v>
+        <v>20150970</v>
       </c>
       <c r="B47" t="s">
         <v>138</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>20170971</v>
+        <v>20150971</v>
       </c>
       <c r="B48" t="s">
         <v>139</v>
@@ -2232,7 +2232,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>20170972</v>
+        <v>20150972</v>
       </c>
       <c r="B49" t="s">
         <v>140</v>
@@ -2261,7 +2261,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>20170973</v>
+        <v>20150973</v>
       </c>
       <c r="B50" t="s">
         <v>141</v>
@@ -2290,7 +2290,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>20170974</v>
+        <v>20150974</v>
       </c>
       <c r="B51" t="s">
         <v>142</v>
@@ -2319,7 +2319,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>20170975</v>
+        <v>20150975</v>
       </c>
       <c r="B52" t="s">
         <v>143</v>
@@ -2348,7 +2348,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>20170976</v>
+        <v>20150976</v>
       </c>
       <c r="B53" t="s">
         <v>144</v>
@@ -2377,7 +2377,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>20170977</v>
+        <v>20150977</v>
       </c>
       <c r="B54" t="s">
         <v>145</v>
@@ -2406,7 +2406,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>20170978</v>
+        <v>20150978</v>
       </c>
       <c r="B55" t="s">
         <v>146</v>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>20170979</v>
+        <v>20150979</v>
       </c>
       <c r="B56" t="s">
         <v>147</v>
@@ -2464,7 +2464,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>20170980</v>
+        <v>20150980</v>
       </c>
       <c r="B57" t="s">
         <v>148</v>
@@ -2493,7 +2493,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>20170981</v>
+        <v>20150981</v>
       </c>
       <c r="B58" t="s">
         <v>149</v>
@@ -2522,7 +2522,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>20170982</v>
+        <v>20150982</v>
       </c>
       <c r="B59" t="s">
         <v>150</v>
@@ -2551,7 +2551,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>20170983</v>
+        <v>20150983</v>
       </c>
       <c r="B60" t="s">
         <v>151</v>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>20170984</v>
+        <v>20150984</v>
       </c>
       <c r="B61" t="s">
         <v>152</v>
@@ -2609,7 +2609,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>20170985</v>
+        <v>20150985</v>
       </c>
       <c r="B62" t="s">
         <v>153</v>
@@ -2638,7 +2638,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>20170986</v>
+        <v>20150986</v>
       </c>
       <c r="B63" t="s">
         <v>154</v>

</xml_diff>

<commit_message>
correction fichier excel non ouvrable sans aucune raison valable
</commit_message>
<xml_diff>
--- a/projetS5/public/INFO/2018-2019/ADMIN/LISTES/INFO_2018-2019_ADMIN_LISTES_S1.xlsx
+++ b/projetS5/public/INFO/2018-2019/ADMIN/LISTES/INFO_2018-2019_ADMIN_LISTES_S1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdcde\Music\PROJET S5 LPDIOC GESTION ETUDIANT\GestionEtudiants2018\projetS5\public\INFO\2018-2019\ADMIN\LISTES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9845B431-76D7-4349-9FF9-E8F9C8FA7A91}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AFD7CD-27C8-4DB7-96CF-40173A3832D5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{B8C28436-09AF-4DF1-8BB7-62D1DDCC6DAF}"/>
   </bookViews>
@@ -856,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A245600-A942-4A9C-BA06-5CDF207C8B57}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C63"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -898,7 +898,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>20150926</v>
+        <v>20170926</v>
       </c>
       <c r="B3" t="s">
         <v>95</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>20150927</v>
+        <v>20170927</v>
       </c>
       <c r="B4" t="s">
         <v>96</v>
@@ -956,7 +956,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>20150928</v>
+        <v>20170928</v>
       </c>
       <c r="B5" t="s">
         <v>97</v>
@@ -985,7 +985,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>20150929</v>
+        <v>20170929</v>
       </c>
       <c r="B6" t="s">
         <v>98</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>20150930</v>
+        <v>20170930</v>
       </c>
       <c r="B7" t="s">
         <v>99</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>20150931</v>
+        <v>20170931</v>
       </c>
       <c r="B8" t="s">
         <v>100</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>20150932</v>
+        <v>20170932</v>
       </c>
       <c r="B9" t="s">
         <v>101</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>20150933</v>
+        <v>20170933</v>
       </c>
       <c r="B10" t="s">
         <v>102</v>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>20150934</v>
+        <v>20170934</v>
       </c>
       <c r="B11" t="s">
         <v>103</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>20150935</v>
+        <v>20170935</v>
       </c>
       <c r="B12" t="s">
         <v>104</v>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>20150936</v>
+        <v>20170936</v>
       </c>
       <c r="B13" t="s">
         <v>105</v>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>20150937</v>
+        <v>20170937</v>
       </c>
       <c r="B14" t="s">
         <v>106</v>
@@ -1246,7 +1246,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>20150938</v>
+        <v>20170938</v>
       </c>
       <c r="B15" t="s">
         <v>107</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>20150939</v>
+        <v>20170939</v>
       </c>
       <c r="B16" t="s">
         <v>108</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>20150940</v>
+        <v>20170940</v>
       </c>
       <c r="B17" t="s">
         <v>109</v>
@@ -1333,7 +1333,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>20150941</v>
+        <v>20170941</v>
       </c>
       <c r="B18" t="s">
         <v>110</v>
@@ -1362,7 +1362,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>20150942</v>
+        <v>20170942</v>
       </c>
       <c r="B19" t="s">
         <v>111</v>
@@ -1391,7 +1391,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>20150943</v>
+        <v>20170943</v>
       </c>
       <c r="B20" t="s">
         <v>112</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>20150944</v>
+        <v>20170944</v>
       </c>
       <c r="B21" t="s">
         <v>113</v>
@@ -1449,7 +1449,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>20150945</v>
+        <v>20170945</v>
       </c>
       <c r="B22" t="s">
         <v>114</v>
@@ -1478,7 +1478,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>20150946</v>
+        <v>20170946</v>
       </c>
       <c r="B23" t="s">
         <v>115</v>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>20150947</v>
+        <v>20170947</v>
       </c>
       <c r="B24" t="s">
         <v>116</v>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>20150948</v>
+        <v>20170948</v>
       </c>
       <c r="B25" t="s">
         <v>117</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>20150949</v>
+        <v>20170949</v>
       </c>
       <c r="B26" t="s">
         <v>118</v>
@@ -1594,7 +1594,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>20150950</v>
+        <v>20170950</v>
       </c>
       <c r="B27" t="s">
         <v>119</v>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>20150951</v>
+        <v>20170951</v>
       </c>
       <c r="B28" t="s">
         <v>120</v>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>20150952</v>
+        <v>20170952</v>
       </c>
       <c r="B29" t="s">
         <v>121</v>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>20150953</v>
+        <v>20170953</v>
       </c>
       <c r="B30" t="s">
         <v>122</v>
@@ -1710,7 +1710,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>20150954</v>
+        <v>20170954</v>
       </c>
       <c r="B31" t="s">
         <v>122</v>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>20150955</v>
+        <v>20170955</v>
       </c>
       <c r="B32" t="s">
         <v>123</v>
@@ -1768,7 +1768,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>20150956</v>
+        <v>20170956</v>
       </c>
       <c r="B33" t="s">
         <v>124</v>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>20150957</v>
+        <v>20170957</v>
       </c>
       <c r="B34" t="s">
         <v>125</v>
@@ -1826,7 +1826,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>20150958</v>
+        <v>20170958</v>
       </c>
       <c r="B35" t="s">
         <v>126</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>20150959</v>
+        <v>20170959</v>
       </c>
       <c r="B36" t="s">
         <v>127</v>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>20150960</v>
+        <v>20170960</v>
       </c>
       <c r="B37" t="s">
         <v>128</v>
@@ -1913,7 +1913,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>20150961</v>
+        <v>20170961</v>
       </c>
       <c r="B38" t="s">
         <v>129</v>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>20150962</v>
+        <v>20170962</v>
       </c>
       <c r="B39" t="s">
         <v>130</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>20150963</v>
+        <v>20170963</v>
       </c>
       <c r="B40" t="s">
         <v>131</v>
@@ -2000,7 +2000,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>20150964</v>
+        <v>20170964</v>
       </c>
       <c r="B41" t="s">
         <v>132</v>
@@ -2029,7 +2029,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>20150965</v>
+        <v>20170965</v>
       </c>
       <c r="B42" t="s">
         <v>133</v>
@@ -2058,7 +2058,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>20150966</v>
+        <v>20170966</v>
       </c>
       <c r="B43" t="s">
         <v>134</v>
@@ -2087,7 +2087,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>20150967</v>
+        <v>20170967</v>
       </c>
       <c r="B44" t="s">
         <v>135</v>
@@ -2116,7 +2116,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>20150968</v>
+        <v>20170968</v>
       </c>
       <c r="B45" t="s">
         <v>136</v>
@@ -2145,7 +2145,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>20150969</v>
+        <v>20170969</v>
       </c>
       <c r="B46" t="s">
         <v>137</v>
@@ -2174,7 +2174,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>20150970</v>
+        <v>20170970</v>
       </c>
       <c r="B47" t="s">
         <v>138</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>20150971</v>
+        <v>20170971</v>
       </c>
       <c r="B48" t="s">
         <v>139</v>
@@ -2232,7 +2232,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>20150972</v>
+        <v>20170972</v>
       </c>
       <c r="B49" t="s">
         <v>140</v>
@@ -2261,7 +2261,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>20150973</v>
+        <v>20170973</v>
       </c>
       <c r="B50" t="s">
         <v>141</v>
@@ -2290,7 +2290,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>20150974</v>
+        <v>20170974</v>
       </c>
       <c r="B51" t="s">
         <v>142</v>
@@ -2319,7 +2319,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>20150975</v>
+        <v>20170975</v>
       </c>
       <c r="B52" t="s">
         <v>143</v>
@@ -2348,7 +2348,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>20150976</v>
+        <v>20170976</v>
       </c>
       <c r="B53" t="s">
         <v>144</v>
@@ -2377,7 +2377,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>20150977</v>
+        <v>20170977</v>
       </c>
       <c r="B54" t="s">
         <v>145</v>
@@ -2406,7 +2406,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>20150978</v>
+        <v>20170978</v>
       </c>
       <c r="B55" t="s">
         <v>146</v>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>20150979</v>
+        <v>20170979</v>
       </c>
       <c r="B56" t="s">
         <v>147</v>
@@ -2464,7 +2464,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>20150980</v>
+        <v>20170980</v>
       </c>
       <c r="B57" t="s">
         <v>148</v>
@@ -2493,7 +2493,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>20150981</v>
+        <v>20170981</v>
       </c>
       <c r="B58" t="s">
         <v>149</v>
@@ -2522,7 +2522,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>20150982</v>
+        <v>20170982</v>
       </c>
       <c r="B59" t="s">
         <v>150</v>
@@ -2551,7 +2551,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>20150983</v>
+        <v>20170983</v>
       </c>
       <c r="B60" t="s">
         <v>151</v>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>20150984</v>
+        <v>20170984</v>
       </c>
       <c r="B61" t="s">
         <v>152</v>
@@ -2609,7 +2609,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>20150985</v>
+        <v>20170985</v>
       </c>
       <c r="B62" t="s">
         <v>153</v>
@@ -2638,7 +2638,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>20150986</v>
+        <v>20170986</v>
       </c>
       <c r="B63" t="s">
         <v>154</v>

</xml_diff>